<commit_message>
store module test added
</commit_message>
<xml_diff>
--- a/Test Data/testdata.xlsx
+++ b/Test Data/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sairam\eclipse-workspace\PetStoreAPIautomation\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EE4C50-1063-4907-A4BF-3973FE10B267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDAD971-2C1C-43C1-A28C-6E18553ED8A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="1455" windowWidth="15375" windowHeight="7875" xr2:uid="{A5A633C0-0C20-4FF6-835D-ADC213D405C2}"/>
+    <workbookView xWindow="4110" yWindow="1320" windowWidth="15375" windowHeight="8010" activeTab="1" xr2:uid="{A5A633C0-0C20-4FF6-835D-ADC213D405C2}"/>
   </bookViews>
   <sheets>
     <sheet name="userdata" sheetId="1" r:id="rId1"/>
+    <sheet name="Storedata" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t>UserID</t>
   </si>
@@ -155,6 +156,39 @@
   </si>
   <si>
     <t>HOBI</t>
+  </si>
+  <si>
+    <t>OrderId</t>
+  </si>
+  <si>
+    <t>petId</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Shipdate</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>2023-11-03T05:42:06.082Z</t>
+  </si>
+  <si>
+    <t>placed</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>conformed</t>
+  </si>
+  <si>
+    <t>cancelled</t>
   </si>
 </sst>
 </file>
@@ -192,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +236,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -219,12 +259,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -542,7 +583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B7CBCF1-2CE4-4159-9EAE-5D580C2585E1}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -760,4 +801,144 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED552D9F-B871-46F3-996E-3916A4189B40}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>123</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>89</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>75</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>